<commit_message>
Aula 08-12 pré aula
</commit_message>
<xml_diff>
--- a/Professor/Material de Acompanhamento_v3.xlsx
+++ b/Professor/Material de Acompanhamento_v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="9" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="20" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="17" state="hidden" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="31" sheetId="13" state="hidden" r:id="rId7"/>
     <sheet name="37 " sheetId="7" state="hidden" r:id="rId8"/>
     <sheet name="33" sheetId="6" state="hidden" r:id="rId9"/>
-    <sheet name="Aula 3" sheetId="23" r:id="rId10"/>
+    <sheet name="Aula 4" sheetId="23" state="hidden" r:id="rId10"/>
     <sheet name="37" sheetId="20" state="hidden" r:id="rId11"/>
     <sheet name="40" sheetId="5" state="hidden" r:id="rId12"/>
     <sheet name="29" sheetId="12" state="hidden" r:id="rId13"/>
@@ -32,18 +32,20 @@
     <sheet name="49-50" sheetId="24" state="hidden" r:id="rId18"/>
     <sheet name="51" sheetId="14" state="hidden" r:id="rId19"/>
     <sheet name="53" sheetId="27" state="hidden" r:id="rId20"/>
-    <sheet name="56" sheetId="39" r:id="rId21"/>
-    <sheet name="57" sheetId="29" r:id="rId22"/>
-    <sheet name="58" sheetId="30" r:id="rId23"/>
-    <sheet name="59" sheetId="33" r:id="rId24"/>
-    <sheet name="60" sheetId="32" r:id="rId25"/>
-    <sheet name="61" sheetId="34" r:id="rId26"/>
-    <sheet name="62" sheetId="36" r:id="rId27"/>
-    <sheet name="64" sheetId="37" r:id="rId28"/>
-    <sheet name="66" sheetId="38" r:id="rId29"/>
-    <sheet name="67" sheetId="40" r:id="rId30"/>
+    <sheet name="Aula 5" sheetId="41" r:id="rId21"/>
+    <sheet name="56" sheetId="39" state="hidden" r:id="rId22"/>
+    <sheet name="57" sheetId="29" state="hidden" r:id="rId23"/>
+    <sheet name="60" sheetId="32" state="hidden" r:id="rId24"/>
+    <sheet name="59" sheetId="33" state="hidden" r:id="rId25"/>
+    <sheet name="65" sheetId="42" r:id="rId26"/>
+    <sheet name="66" sheetId="38" r:id="rId27"/>
+    <sheet name="67" sheetId="40" r:id="rId28"/>
+    <sheet name="58" sheetId="30" r:id="rId29"/>
+    <sheet name="61" sheetId="34" r:id="rId30"/>
+    <sheet name="62" sheetId="36" r:id="rId31"/>
+    <sheet name="64" sheetId="37" r:id="rId32"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="310">
   <si>
     <t>Lista de Compras</t>
   </si>
@@ -929,10 +931,85 @@
     <t>NÂO MENCIONAR PREÇO PONDERADO</t>
   </si>
   <si>
-    <t>Para quem acabar, pedir para formatar.</t>
-  </si>
-  <si>
-    <t>Pedir para mudar core formatar, mudar fonte</t>
+    <t>Função SE</t>
+  </si>
+  <si>
+    <t>Função Aninhada</t>
+  </si>
+  <si>
+    <t>Filtro Avançado</t>
+  </si>
+  <si>
+    <t>Fornecedor Direite, Esquerda, Etx Texto</t>
+  </si>
+  <si>
+    <t>Fornecedores</t>
+  </si>
+  <si>
+    <t>Remover Duplicatas</t>
+  </si>
+  <si>
+    <t>Relembrar como Fazer Grafico - DRE</t>
+  </si>
+  <si>
+    <t>grafico: Tendencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrir Arquivo DRE e </t>
+  </si>
+  <si>
+    <t>REFAZER O GRAFICO RAPIDAMENTE</t>
+  </si>
+  <si>
+    <t>Mosatar a formatação rapidamente.</t>
+  </si>
+  <si>
+    <t>Brincar com grafico e Projeções IBGE</t>
+  </si>
+  <si>
+    <t>ELIMINAR DUPLICATAS</t>
+  </si>
+  <si>
+    <t>Arquivo VENDAS RESOLVIDO.xlxs</t>
+  </si>
+  <si>
+    <t>Mostrar ELIMINAR DUPLICATAS .</t>
+  </si>
+  <si>
+    <t>MOSTRAR TRABALHGAR EM CONJUNTO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - COM SOMASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - MEDIA SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - GRAFICO</t>
+  </si>
+  <si>
+    <t>Correção do Exercicio Forncedores</t>
+  </si>
+  <si>
+    <t>Brincar com Grafico BGE e FAZER Grafico Homem x Mulher</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Exercicios SE</t>
+  </si>
+  <si>
+    <t>Correção Exercicios</t>
+  </si>
+  <si>
+    <t>Explicação Classficiação LISTA PERSONALIZADA</t>
+  </si>
+  <si>
+    <t>Exercicios Lista Personalizada - Esquerda/Direita</t>
+  </si>
+  <si>
+    <t>Explicação Formatação SIMPLES</t>
   </si>
 </sst>
 </file>
@@ -2172,7 +2249,7 @@
   <dimension ref="A2:H36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3934,10 +4011,513 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="50.85546875" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D4" s="12">
+        <f>C4-B4</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B5" s="12">
+        <f>C4</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" ref="D5:D18" si="0">C5-B5</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F5" s="15">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="B6" s="12">
+        <f>C5</f>
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>294</v>
+      </c>
+      <c r="F6" s="15">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12">
+        <f>C6</f>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
+        <v>3.4722222222222265E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>287</v>
+      </c>
+      <c r="F7" s="15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" ref="B8:B10" si="1">C7</f>
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>302</v>
+      </c>
+      <c r="F8" s="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F9" s="15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B10" s="12">
+        <f t="shared" si="1"/>
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555525E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="B11" s="12">
+        <f>C10</f>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="B12" s="12">
+        <f t="shared" ref="B12:B15" si="2">C11</f>
+        <v>0.5625</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>305</v>
+      </c>
+      <c r="F12" s="15">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B13" s="12">
+        <f t="shared" si="2"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="0"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>306</v>
+      </c>
+      <c r="F13" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" si="2"/>
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="0"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>307</v>
+      </c>
+      <c r="F14" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="0"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>308</v>
+      </c>
+      <c r="F15" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B16" s="12">
+        <f>C15</f>
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="0"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B17" s="12">
+        <f>C16</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="0"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>309</v>
+      </c>
+      <c r="F17" s="15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B18" s="12">
+        <f>C17</f>
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="0"/>
+        <v>3.4722222222220989E-3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>263</v>
+      </c>
+      <c r="F18" s="15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="23"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="23"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="B3:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,12 +4552,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="B3:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4018,7 +4601,218 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="B3:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>281</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F23"/>
   <sheetViews>
@@ -4105,304 +4899,6 @@
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>235</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>281</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>232</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>274</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -4457,25 +4953,175 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B5"/>
+  <dimension ref="B2:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>284</v>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>274</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aula 16-12 pre aula
</commit_message>
<xml_diff>
--- a/Professor/Material de Acompanhamento_v3.xlsx
+++ b/Professor/Material de Acompanhamento_v3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u100054\Desktop\aprendizado\Aulas Excel Basico\Fenrir\Professor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Empreendedor\Aulas Excel Basico\fenrir\Professor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="20" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="36" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="17" state="hidden" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <sheet name="49-50" sheetId="24" state="hidden" r:id="rId18"/>
     <sheet name="51" sheetId="14" state="hidden" r:id="rId19"/>
     <sheet name="53" sheetId="27" state="hidden" r:id="rId20"/>
-    <sheet name="Aula 5" sheetId="41" r:id="rId21"/>
+    <sheet name="Aula 5" sheetId="41" state="hidden" r:id="rId21"/>
     <sheet name="56" sheetId="39" state="hidden" r:id="rId22"/>
     <sheet name="57" sheetId="29" state="hidden" r:id="rId23"/>
     <sheet name="60" sheetId="32" state="hidden" r:id="rId24"/>
@@ -40,19 +40,21 @@
     <sheet name="58" sheetId="30" state="hidden" r:id="rId26"/>
     <sheet name="62" sheetId="36" state="hidden" r:id="rId27"/>
     <sheet name="64" sheetId="37" state="hidden" r:id="rId28"/>
-    <sheet name="65" sheetId="42" r:id="rId29"/>
-    <sheet name="66" sheetId="38" r:id="rId30"/>
-    <sheet name="67" sheetId="46" r:id="rId31"/>
-    <sheet name="68" sheetId="40" r:id="rId32"/>
-    <sheet name="69" sheetId="51" r:id="rId33"/>
-    <sheet name="71" sheetId="34" r:id="rId34"/>
-    <sheet name="73" sheetId="48" r:id="rId35"/>
-    <sheet name="74" sheetId="50" r:id="rId36"/>
-    <sheet name="75" sheetId="52" r:id="rId37"/>
-    <sheet name="72" sheetId="47" r:id="rId38"/>
-    <sheet name="76" sheetId="53" r:id="rId39"/>
+    <sheet name="65" sheetId="42" state="hidden" r:id="rId29"/>
+    <sheet name="66" sheetId="38" state="hidden" r:id="rId30"/>
+    <sheet name="67" sheetId="46" state="hidden" r:id="rId31"/>
+    <sheet name="68" sheetId="40" state="hidden" r:id="rId32"/>
+    <sheet name="69" sheetId="51" state="hidden" r:id="rId33"/>
+    <sheet name="71" sheetId="34" state="hidden" r:id="rId34"/>
+    <sheet name="73" sheetId="48" state="hidden" r:id="rId35"/>
+    <sheet name="74" sheetId="50" state="hidden" r:id="rId36"/>
+    <sheet name="Aula 6" sheetId="54" r:id="rId37"/>
+    <sheet name="75" sheetId="52" r:id="rId38"/>
+    <sheet name="72" sheetId="47" r:id="rId39"/>
+    <sheet name="76" sheetId="53" r:id="rId40"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="345">
   <si>
     <t>Lista de Compras</t>
   </si>
@@ -1113,6 +1115,15 @@
   </si>
   <si>
     <t>Filtro avançado</t>
+  </si>
+  <si>
+    <t>Relembrar explicação do SE</t>
+  </si>
+  <si>
+    <t>Exercicio se</t>
+  </si>
+  <si>
+    <t>Correção do SE</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1230,6 +1241,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1243,7 +1260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1275,6 +1292,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1819,7 +1837,7 @@
         <v>0.47569444444444442</v>
       </c>
       <c r="D13" s="12">
-        <f t="shared" ref="D13" si="1">C13-B13</f>
+        <f>C13-B13</f>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="E13" t="s">
@@ -1982,7 +2000,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D20" s="12">
-        <f t="shared" ref="D20:D21" si="2">C20-B20</f>
+        <f t="shared" ref="D20:D35" si="1">C20-B20</f>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="E20" t="s">
@@ -2000,7 +2018,7 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="D21" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E21" t="s">
@@ -2024,7 +2042,7 @@
         <v>0.61111111111111105</v>
       </c>
       <c r="D22" s="12">
-        <f t="shared" ref="D22" si="3">C22-B22</f>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E22" t="s">
@@ -2048,7 +2066,7 @@
         <v>0.61805555555555558</v>
       </c>
       <c r="D23" s="12">
-        <f t="shared" ref="D23:D24" si="4">C23-B23</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="E23" t="s">
@@ -2072,7 +2090,7 @@
         <v>0.63194444444444442</v>
       </c>
       <c r="D24" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E24" t="s">
@@ -2096,7 +2114,7 @@
         <v>0.65277777777777779</v>
       </c>
       <c r="D25" s="12">
-        <f t="shared" ref="D25" si="5">C25-B25</f>
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E25" t="s">
@@ -2120,7 +2138,7 @@
         <v>0.65972222222222221</v>
       </c>
       <c r="D26" s="12">
-        <f t="shared" ref="D26:D28" si="6">C26-B26</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E26" t="s">
@@ -2144,7 +2162,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D27" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E27" t="s">
@@ -2168,7 +2186,7 @@
         <v>0.67361111111111116</v>
       </c>
       <c r="D28" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="E28" t="s">
@@ -2192,7 +2210,7 @@
         <v>0.68402777777777779</v>
       </c>
       <c r="D29" s="12">
-        <f t="shared" ref="D29" si="7">C29-B29</f>
+        <f t="shared" si="1"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="E29" t="s">
@@ -2216,7 +2234,7 @@
         <v>0.70138888888888884</v>
       </c>
       <c r="D30" s="12">
-        <f t="shared" ref="D30" si="8">C30-B30</f>
+        <f t="shared" si="1"/>
         <v>1.7361111111111049E-2</v>
       </c>
       <c r="E30" t="s">
@@ -2240,7 +2258,7 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D31" s="12">
-        <f t="shared" ref="D31" si="9">C31-B31</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="E31" t="s">
@@ -2264,7 +2282,7 @@
         <v>0.71527777777777779</v>
       </c>
       <c r="D32" s="12">
-        <f t="shared" ref="D32:D33" si="10">C32-B32</f>
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E32" t="s">
@@ -2288,7 +2306,7 @@
         <v>0.72222222222222221</v>
       </c>
       <c r="D33" s="12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="E33" t="s">
@@ -2312,7 +2330,7 @@
         <v>0.74305555555555547</v>
       </c>
       <c r="D34" s="12">
-        <f t="shared" ref="D34:D35" si="11">C34-B34</f>
+        <f t="shared" si="1"/>
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="E34" t="s">
@@ -2336,7 +2354,7 @@
         <v>0.75</v>
       </c>
       <c r="D35" s="12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="1"/>
         <v>6.9444444444445308E-3</v>
       </c>
       <c r="E35" t="s">
@@ -2424,14 +2442,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="B5" s="12">
-        <f>C4</f>
+        <f t="shared" ref="B5:B10" si="0">C4</f>
         <v>0.3611111111111111</v>
       </c>
       <c r="C5" s="12">
         <v>0.38194444444444442</v>
       </c>
       <c r="D5" s="12">
-        <f t="shared" ref="D5:D16" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D16" si="1">C5-B5</f>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E5" t="s">
@@ -2446,14 +2464,14 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="B6" s="12">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>0.38194444444444442</v>
       </c>
       <c r="C6" s="12">
         <v>0.41666666666666669</v>
       </c>
       <c r="D6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.4722222222222265E-2</v>
       </c>
       <c r="E6" t="s">
@@ -2466,14 +2484,14 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="C7" s="12">
         <v>0.43055555555555558</v>
       </c>
       <c r="D7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="E7" t="s">
@@ -2488,14 +2506,14 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B8" s="12">
-        <f t="shared" ref="B8:B9" si="1">C7</f>
+        <f t="shared" si="0"/>
         <v>0.43055555555555558</v>
       </c>
       <c r="C8" s="12">
         <v>0.4513888888888889</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E8" t="s">
@@ -2510,14 +2528,14 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4513888888888889</v>
       </c>
       <c r="C9" s="12">
         <v>0.46180555555555558</v>
       </c>
       <c r="D9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="E9" t="s">
@@ -2532,14 +2550,14 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B10" s="12">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>0.46180555555555558</v>
       </c>
       <c r="C10" s="12">
         <v>0.48958333333333331</v>
       </c>
       <c r="D10" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.7777777777777735E-2</v>
       </c>
       <c r="E10" t="s">
@@ -2560,7 +2578,7 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.2083333333333315E-2</v>
       </c>
       <c r="E11" t="s">
@@ -2572,14 +2590,14 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="B12" s="12">
-        <f t="shared" ref="B12:B15" si="2">C11</f>
+        <f t="shared" ref="B12:B18" si="2">C11</f>
         <v>0.54166666666666663</v>
       </c>
       <c r="C12" s="12">
         <v>0.55555555555555558</v>
       </c>
       <c r="D12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="E12" t="s">
@@ -2601,7 +2619,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E13" t="s">
@@ -2623,7 +2641,7 @@
         <v>0.59722222222222221</v>
       </c>
       <c r="D14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E14" t="s">
@@ -2645,7 +2663,7 @@
         <v>0.625</v>
       </c>
       <c r="D15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E15" t="s">
@@ -2660,14 +2678,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B16" s="12">
-        <f>C15</f>
+        <f t="shared" si="2"/>
         <v>0.625</v>
       </c>
       <c r="C16" s="12">
         <v>0.64583333333333337</v>
       </c>
       <c r="D16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E16" t="s">
@@ -2682,14 +2700,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B17" s="12">
-        <f>C16</f>
+        <f t="shared" si="2"/>
         <v>0.64583333333333337</v>
       </c>
       <c r="C17" s="12">
         <v>0.66666666666666663</v>
       </c>
       <c r="D17" s="12">
-        <f t="shared" ref="D17" si="3">C17-B17</f>
+        <f>C17-B17</f>
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="E17" t="s">
@@ -2704,14 +2722,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B18" s="12">
-        <f>C17</f>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="C18" s="12">
         <v>0.68055555555555547</v>
       </c>
       <c r="D18" s="12">
-        <f t="shared" ref="D18" si="4">C18-B18</f>
+        <f>C18-B18</f>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E18" t="s">
@@ -4123,8 +4141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,14 +4207,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="B5" s="12">
-        <f>C4</f>
+        <f t="shared" ref="B5:B13" si="0">C4</f>
         <v>0.3611111111111111</v>
       </c>
       <c r="C5" s="12">
         <v>0.375</v>
       </c>
       <c r="D5" s="12">
-        <f t="shared" ref="D5:D20" si="0">C5-B5</f>
+        <f t="shared" ref="D5:D20" si="1">C5-B5</f>
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="E5" t="s">
@@ -4211,14 +4229,14 @@
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="B6" s="12">
-        <f>C5</f>
+        <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
       <c r="C6" s="12">
         <v>0.39583333333333331</v>
       </c>
       <c r="D6" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0833333333333315E-2</v>
       </c>
       <c r="E6" t="s">
@@ -4231,14 +4249,14 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12">
-        <f>C6</f>
+        <f t="shared" si="0"/>
         <v>0.39583333333333331</v>
       </c>
       <c r="C7" s="12">
         <v>0.40972222222222227</v>
       </c>
       <c r="D7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="E7" t="s">
@@ -4253,14 +4271,14 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B8" s="12">
-        <f t="shared" ref="B8:B9" si="1">C7</f>
+        <f t="shared" si="0"/>
         <v>0.40972222222222227</v>
       </c>
       <c r="C8" s="12">
         <v>0.4236111111111111</v>
       </c>
       <c r="D8" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E8" t="s">
@@ -4275,14 +4293,14 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B9" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.4236111111111111</v>
       </c>
       <c r="C9" s="12">
         <v>0.47222222222222227</v>
       </c>
       <c r="D9" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.861111111111116E-2</v>
       </c>
       <c r="E9" t="s">
@@ -4297,7 +4315,7 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B10" s="12">
-        <f t="shared" ref="B10" si="2">C9</f>
+        <f t="shared" si="0"/>
         <v>0.47222222222222227</v>
       </c>
       <c r="C10" s="12">
@@ -4319,14 +4337,14 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B11" s="12">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>0.49305555555555558</v>
       </c>
       <c r="C11" s="12">
         <v>0.54166666666666663</v>
       </c>
       <c r="D11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.8611111111111049E-2</v>
       </c>
       <c r="E11" t="s">
@@ -4338,14 +4356,14 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B12" s="12">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>0.54166666666666663</v>
       </c>
       <c r="C12" s="12">
         <v>0.58333333333333337</v>
       </c>
       <c r="D12" s="12">
-        <f t="shared" ref="D12" si="3">C12-B12</f>
+        <f>C12-B12</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="E12" t="s">
@@ -4360,14 +4378,14 @@
         <v>1.388888888888884E-2</v>
       </c>
       <c r="B13" s="12">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="C13" s="12">
         <v>0.60416666666666663</v>
       </c>
       <c r="D13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0833333333333259E-2</v>
       </c>
       <c r="E13" t="s">
@@ -4382,14 +4400,14 @@
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="B14" s="12">
-        <f t="shared" ref="B14:B20" si="4">C13</f>
+        <f t="shared" ref="B14:B20" si="2">C13</f>
         <v>0.60416666666666663</v>
       </c>
       <c r="C14" s="12">
         <v>0.61805555555555558</v>
       </c>
       <c r="D14" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="E14" t="s">
@@ -4404,14 +4422,14 @@
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B15" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.61805555555555558</v>
       </c>
       <c r="C15" s="12">
         <v>0.63888888888888895</v>
       </c>
       <c r="D15" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E15" t="s">
@@ -4426,14 +4444,14 @@
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="B16" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.63888888888888895</v>
       </c>
       <c r="C16" s="12">
         <v>0.65277777777777779</v>
       </c>
       <c r="D16" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E16" t="s">
@@ -4448,14 +4466,14 @@
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B17" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.65277777777777779</v>
       </c>
       <c r="C17" s="12">
         <v>0.66666666666666663</v>
       </c>
       <c r="D17" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E17" t="s">
@@ -4470,14 +4488,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B18" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="C18" s="12">
         <v>0.6875</v>
       </c>
       <c r="D18" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E18" t="s">
@@ -4492,14 +4510,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B19" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.6875</v>
       </c>
       <c r="C19" s="12">
         <v>0.70138888888888884</v>
       </c>
       <c r="D19" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.388888888888884E-2</v>
       </c>
       <c r="E19" t="s">
@@ -4514,14 +4532,14 @@
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B20" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>0.70138888888888884</v>
       </c>
       <c r="C20" s="12">
         <v>0.68055555555555547</v>
       </c>
       <c r="D20" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.083333333333337E-2</v>
       </c>
     </row>
@@ -4617,7 +4635,7 @@
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
-      <c r="E32" t="s">
+      <c r="E32" s="29" t="s">
         <v>333</v>
       </c>
     </row>
@@ -4626,7 +4644,7 @@
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
-      <c r="E33" t="s">
+      <c r="E33" s="29" t="s">
         <v>334</v>
       </c>
     </row>
@@ -4635,7 +4653,7 @@
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
-      <c r="E34" t="s">
+      <c r="E34" s="29" t="s">
         <v>335</v>
       </c>
     </row>
@@ -4644,7 +4662,7 @@
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="E35" t="s">
+      <c r="E35" s="29" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4653,7 +4671,7 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="E36" t="s">
+      <c r="E36" s="29" t="s">
         <v>336</v>
       </c>
     </row>
@@ -4662,7 +4680,7 @@
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="E37" t="s">
+      <c r="E37" s="29" t="s">
         <v>337</v>
       </c>
     </row>
@@ -4671,17 +4689,17 @@
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
-      <c r="E38" t="s">
+      <c r="E38" s="29" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
+      <c r="E39" s="29" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
+      <c r="E40" s="29" t="s">
         <v>341</v>
       </c>
     </row>
@@ -5233,7 +5251,7 @@
   <dimension ref="B1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5271,7 +5289,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5316,7 +5334,7 @@
   <dimension ref="B3:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,7 +5430,7 @@
   <dimension ref="B3:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5438,7 +5456,7 @@
   <dimension ref="B2:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5464,7 +5482,7 @@
   <dimension ref="B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5487,7 +5505,7 @@
   <dimension ref="B3:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5512,6 +5530,578 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="50.85546875" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D4" s="12">
+        <f>C4-B4</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B5" s="12">
+        <f t="shared" ref="B5:B20" si="0">C4</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" ref="D5:D20" si="1">C5-B5</f>
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>342</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>343</v>
+      </c>
+      <c r="F6" s="15">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="1"/>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>344</v>
+      </c>
+      <c r="F7" s="15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" si="0"/>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="1"/>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>328</v>
+      </c>
+      <c r="F8" s="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" si="0"/>
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="1"/>
+        <v>4.861111111111116E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F9" s="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B10" s="12">
+        <f t="shared" si="0"/>
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="D10" s="12">
+        <f>C10-B10</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+      <c r="F10" s="15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B11" s="12">
+        <f t="shared" si="0"/>
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="1"/>
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B12" s="12">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D12" s="12">
+        <f>C12-B12</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>317</v>
+      </c>
+      <c r="F12" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="B13" s="12">
+        <f t="shared" si="0"/>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>298</v>
+      </c>
+      <c r="F13" s="15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>299</v>
+      </c>
+      <c r="F14" s="15">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="0"/>
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="1"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>300</v>
+      </c>
+      <c r="F15" s="15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="B16" s="12">
+        <f t="shared" si="0"/>
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="1"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F16" s="15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B17" s="12">
+        <f t="shared" si="0"/>
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="1"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>296</v>
+      </c>
+      <c r="F17" s="15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B18" s="12">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.6875</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="1"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>297</v>
+      </c>
+      <c r="F18" s="15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B19" s="12">
+        <f t="shared" si="0"/>
+        <v>0.6875</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="1"/>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F19" s="15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B20" s="12">
+        <f t="shared" si="0"/>
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="1"/>
+        <v>-2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="23"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="29" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="29" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="29" t="s">
+        <v>341</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D3"/>
   <sheetViews>
@@ -5533,7 +6123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B9"/>
   <sheetViews>
@@ -5570,28 +6160,6 @@
       <c r="B9" t="s">
         <v>325</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>330</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -5699,6 +6267,28 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -5949,55 +6539,55 @@
         <v>0.02</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" ref="D10:D12" si="1">$C$9/C10*$C$4</f>
+        <f>$C$9/C10*$C$4</f>
         <v>158.5</v>
       </c>
       <c r="E10">
-        <f t="shared" ref="E10:P10" si="2">D10*E$6</f>
+        <f t="shared" ref="E10:P10" si="1">D10*E$6</f>
         <v>237750</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>47550000</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10936500000</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2624760000000</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>656190000000000</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.706094E+17</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.6064538E+19</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.2898070640000001E+22</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.7404404856000003E+24</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1221321456800001E+27</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.4786096516080003E+29</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.1131550885145601E+32</v>
       </c>
     </row>
@@ -6009,55 +6599,55 @@
         <v>3.8</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f>$C$9/C11*$C$4</f>
         <v>0.83421052631578951</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:P11" si="3">D11*E$6</f>
+        <f t="shared" ref="E11:P11" si="2">D11*E$6</f>
         <v>1251.3157894736842</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>250263.15789473683</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>57560526.315789469</v>
       </c>
       <c r="H11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>13814526315.789473</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>3453631578947.3682</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>897944210526315.75</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.4244493684210525E+17</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>6.7884582315789468E+19</v>
       </c>
       <c r="M11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.9686528871578947E+22</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.9059586614736843E+24</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1.8308471850568421E+27</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>5.8587109921818949E+29</v>
       </c>
     </row>
@@ -6069,55 +6659,55 @@
         <v>0.3</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f>$C$9/C12*$C$4</f>
         <v>10.566666666666666</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:P12" si="4">D12*E$6</f>
+        <f t="shared" ref="E12:P12" si="3">D12*E$6</f>
         <v>15850</v>
       </c>
       <c r="F12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3170000</v>
       </c>
       <c r="G12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>729100000</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>174984000000</v>
       </c>
       <c r="I12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>43746000000000</v>
       </c>
       <c r="J12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.137396E+16</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.0709692E+18</v>
       </c>
       <c r="L12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8.5987137599999993E+20</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2.4936269903999999E+23</v>
       </c>
       <c r="N12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.4808809711999994E+25</v>
       </c>
       <c r="O12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>2.3190731010719999E+28</v>
       </c>
       <c r="P12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.4210339234303991E+30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aula 22-12 pre aula
</commit_message>
<xml_diff>
--- a/Professor/Material de Acompanhamento_v3.xlsx
+++ b/Professor/Material de Acompanhamento_v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="36" activeTab="36"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="38" activeTab="38"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="17" state="hidden" r:id="rId1"/>
@@ -48,19 +48,23 @@
     <sheet name="71" sheetId="34" state="hidden" r:id="rId34"/>
     <sheet name="73" sheetId="48" state="hidden" r:id="rId35"/>
     <sheet name="74" sheetId="50" state="hidden" r:id="rId36"/>
-    <sheet name="Aula 6" sheetId="54" r:id="rId37"/>
+    <sheet name="Aula 6" sheetId="54" state="hidden" r:id="rId37"/>
     <sheet name="72" sheetId="47" state="hidden" r:id="rId38"/>
-    <sheet name="76" sheetId="52" r:id="rId39"/>
-    <sheet name="77" sheetId="57" r:id="rId40"/>
-    <sheet name="78" sheetId="53" r:id="rId41"/>
-    <sheet name="79" sheetId="55" r:id="rId42"/>
-    <sheet name="80" sheetId="58" r:id="rId43"/>
-    <sheet name="81" sheetId="59" r:id="rId44"/>
-    <sheet name="82" sheetId="60" r:id="rId45"/>
-    <sheet name="83" sheetId="62" r:id="rId46"/>
-    <sheet name="84" sheetId="65" r:id="rId47"/>
+    <sheet name="Aula 7" sheetId="66" r:id="rId39"/>
+    <sheet name="Planilha3" sheetId="68" r:id="rId40"/>
+    <sheet name="76" sheetId="52" state="hidden" r:id="rId41"/>
+    <sheet name="77" sheetId="57" state="hidden" r:id="rId42"/>
+    <sheet name="78" sheetId="53" state="hidden" r:id="rId43"/>
+    <sheet name="79" sheetId="55" state="hidden" r:id="rId44"/>
+    <sheet name="80" sheetId="58" state="hidden" r:id="rId45"/>
+    <sheet name="81" sheetId="59" state="hidden" r:id="rId46"/>
+    <sheet name="82" sheetId="60" state="hidden" r:id="rId47"/>
+    <sheet name="83" sheetId="62" state="hidden" r:id="rId48"/>
+    <sheet name="84" sheetId="65" state="hidden" r:id="rId49"/>
+    <sheet name="85" sheetId="67" r:id="rId50"/>
+    <sheet name="86" sheetId="69" r:id="rId51"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="416">
   <si>
     <t>Lista de Compras</t>
   </si>
@@ -1265,6 +1269,84 @@
   </si>
   <si>
     <t xml:space="preserve"> &gt; fazer exemplo de auditoria com DIAS atrasados x JUROS (aba de boletos).</t>
+  </si>
+  <si>
+    <t>Tabela Dinamica</t>
+  </si>
+  <si>
+    <t>Grafico Dinamico</t>
+  </si>
+  <si>
+    <t>Fonte Externa Dinamica</t>
+  </si>
+  <si>
+    <t>DashBoar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Tabela</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Formatação Condicional</t>
+  </si>
+  <si>
+    <t>Relembrar tabela Dinamica</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -  Mostar Proprieda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Nbão pode ter campos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Nostrar detalhes no numero</t>
+  </si>
+  <si>
+    <t>- Criar campo calculado</t>
+  </si>
+  <si>
+    <t>Demonstar CAMPO CALCULADo</t>
+  </si>
+  <si>
+    <t>Pedir para Calcular CAMPO CALCULADO</t>
+  </si>
+  <si>
+    <t>Mostrar Conciliação</t>
+  </si>
+  <si>
+    <t>Exercicio Conciliaçção</t>
+  </si>
+  <si>
+    <t>Correção da Conciliação</t>
+  </si>
+  <si>
+    <t>Mostrar Grtafico Dinamico</t>
+  </si>
+  <si>
+    <t>Pedir Grafico Dinamicco</t>
+  </si>
+  <si>
+    <t>Mostrar Conexão De dados Dinamica</t>
+  </si>
+  <si>
+    <t>Pedir Demonstração simnples de conexão</t>
+  </si>
+  <si>
+    <t>Exercicios de DAshBoard1</t>
+  </si>
+  <si>
+    <t>Exercicios DashBoard2</t>
+  </si>
+  <si>
+    <t>Imposrtação Dinamica de Arquivo Externo</t>
+  </si>
+  <si>
+    <t>Exercicios Oiportação Externa</t>
+  </si>
+  <si>
+    <t>Mostrar Importação</t>
+  </si>
+  <si>
+    <t>Mostrar Impressão</t>
   </si>
 </sst>
 </file>
@@ -5690,10 +5772,10 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I39"/>
+  <dimension ref="A2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5761,14 +5843,14 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="B5" s="12">
-        <f t="shared" ref="B5:B20" si="0">C4</f>
+        <f t="shared" ref="B5:B19" si="0">C4</f>
         <v>0.3611111111111111</v>
       </c>
       <c r="C5" s="12">
         <v>0.3888888888888889</v>
       </c>
       <c r="D5" s="12">
-        <f t="shared" ref="D5:D20" si="1">C5-B5</f>
+        <f t="shared" ref="D5:D19" si="1">C5-B5</f>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E5" t="s">
@@ -6341,6 +6423,36 @@
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E39" s="29" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -6394,41 +6506,692 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D9"/>
+  <dimension ref="A2:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="50.85546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>352</v>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C4" s="12">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D4" s="12">
+        <f>C4-B4</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="15">
+        <v>75</v>
+      </c>
+      <c r="I4">
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="B5" s="12">
+        <f t="shared" ref="B5:B19" si="0">C4</f>
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.375</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" ref="D5:D19" si="1">C5-B5</f>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>396</v>
+      </c>
+      <c r="F5" s="15">
+        <v>76</v>
+      </c>
+      <c r="I5">
+        <v>6.9444444444444753E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="B6" s="12">
+        <f t="shared" si="0"/>
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="12">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>401</v>
+      </c>
+      <c r="F6" s="15">
+        <v>77</v>
+      </c>
+      <c r="I6">
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12">
+        <f t="shared" si="0"/>
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="1"/>
+        <v>1.7361111111111049E-2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>402</v>
+      </c>
+      <c r="F7" s="15">
+        <v>77</v>
+      </c>
+      <c r="I7">
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" si="0"/>
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>403</v>
+      </c>
+      <c r="F8" s="15">
+        <v>78</v>
+      </c>
+      <c r="I8">
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="1"/>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>404</v>
+      </c>
+      <c r="F9" s="15">
+        <v>79</v>
+      </c>
+      <c r="I9">
+        <v>6.9444444444444198E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B10" s="12">
+        <f t="shared" si="0"/>
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D10" s="12">
+        <f>C10-B10</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F10" s="15">
+        <v>79</v>
+      </c>
+      <c r="I10">
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B11" s="12">
+        <f t="shared" si="0"/>
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0.46875</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>406</v>
+      </c>
+      <c r="F11" s="15">
+        <v>79</v>
+      </c>
+      <c r="I11">
+        <v>6.9444444444444753E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B12" s="12">
+        <f t="shared" si="0"/>
+        <v>0.46875</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D12" s="12">
+        <f>C12-B12</f>
+        <v>2.0833333333333315E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>407</v>
+      </c>
+      <c r="F12" s="15">
+        <v>79</v>
+      </c>
+      <c r="I12">
+        <v>0.13194444444444448</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="B13" s="12">
+        <f t="shared" si="0"/>
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C13" s="12">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="1"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F13" s="15">
+        <v>81</v>
+      </c>
+      <c r="I13">
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="30">
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" si="0"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>408</v>
+      </c>
+      <c r="I14">
+        <v>1.3888888888888951E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="0"/>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C15" s="12">
+        <v>0.5625</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="1"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>409</v>
+      </c>
+      <c r="F15" s="15">
+        <v>82</v>
+      </c>
+      <c r="I15">
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="12">
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="B16" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5625</v>
+      </c>
+      <c r="C16" s="12">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="1"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>410</v>
+      </c>
+      <c r="F16" s="15">
+        <v>82</v>
+      </c>
+      <c r="I16">
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="12">
+        <v>6.9444444444444753E-3</v>
+      </c>
+      <c r="B17" s="12">
+        <f t="shared" si="0"/>
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C17" s="12">
+        <v>0.625</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="1"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>411</v>
+      </c>
+      <c r="F17" s="15">
+        <v>83</v>
+      </c>
+      <c r="I17">
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B18" s="12">
+        <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+      <c r="C18" s="12">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="1"/>
+        <v>1.3888888888888951E-2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>412</v>
+      </c>
+      <c r="F18" s="15">
+        <v>84</v>
+      </c>
+      <c r="I18">
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B19" s="12">
+        <f t="shared" si="0"/>
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C19" s="12">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>413</v>
+      </c>
+      <c r="F19" s="15">
+        <v>84</v>
+      </c>
+      <c r="I19">
+        <v>1.388888888888884E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B20" s="12">
+        <f>C19</f>
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C20" s="12">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D20" s="12">
+        <f>C20-B20</f>
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="15">
+        <v>84</v>
+      </c>
+      <c r="I20">
+        <v>-2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B21" s="12">
+        <f>C20</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C21" s="12">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D21" s="12">
+        <f>C21-B21</f>
+        <v>2.7777777777777901E-2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>414</v>
+      </c>
+      <c r="F21" s="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>2.4305555555555525E-2</v>
+      </c>
+      <c r="B22" s="12">
+        <f>C21</f>
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="C22" s="12">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D22" s="12">
+        <f>C22-B22</f>
+        <v>1.388888888888884E-2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>415</v>
+      </c>
+      <c r="F22" s="15">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+    </row>
+    <row r="32" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>332</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="29" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="29" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="29" t="s">
+        <v>336</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="29" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6535,10 +7298,68 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6555,12 +7376,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6585,12 +7409,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6623,12 +7450,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6652,12 +7482,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B4:E13"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6699,12 +7532,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6723,8 +7559,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6838,7 +7677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
@@ -6942,6 +7781,89 @@
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aula 11-01-19 pre aula
</commit_message>
<xml_diff>
--- a/Professor/Material de Acompanhamento_v3.xlsx
+++ b/Professor/Material de Acompanhamento_v3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u100054\Desktop\aprendizado\Aulas Excel Basico\Fenrir\Professor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Empreendedor\Aulas Excel Basico\fenrir\Professor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="38" activeTab="38"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="673" firstSheet="38" activeTab="54"/>
   </bookViews>
   <sheets>
     <sheet name="Aula 1" sheetId="17" state="hidden" r:id="rId1"/>
@@ -50,20 +50,27 @@
     <sheet name="74" sheetId="50" state="hidden" r:id="rId36"/>
     <sheet name="Aula 6" sheetId="54" state="hidden" r:id="rId37"/>
     <sheet name="72" sheetId="47" state="hidden" r:id="rId38"/>
-    <sheet name="Aula 7" sheetId="66" r:id="rId39"/>
-    <sheet name="Planilha3" sheetId="68" r:id="rId40"/>
-    <sheet name="76" sheetId="52" state="hidden" r:id="rId41"/>
-    <sheet name="77" sheetId="57" state="hidden" r:id="rId42"/>
-    <sheet name="78" sheetId="53" state="hidden" r:id="rId43"/>
-    <sheet name="79" sheetId="55" state="hidden" r:id="rId44"/>
-    <sheet name="80" sheetId="58" state="hidden" r:id="rId45"/>
-    <sheet name="81" sheetId="59" state="hidden" r:id="rId46"/>
-    <sheet name="82" sheetId="60" state="hidden" r:id="rId47"/>
-    <sheet name="83" sheetId="62" state="hidden" r:id="rId48"/>
-    <sheet name="84" sheetId="65" state="hidden" r:id="rId49"/>
-    <sheet name="85" sheetId="67" r:id="rId50"/>
-    <sheet name="86" sheetId="69" r:id="rId51"/>
+    <sheet name="Aula 7" sheetId="70" r:id="rId39"/>
+    <sheet name="76" sheetId="52" state="hidden" r:id="rId40"/>
+    <sheet name="77" sheetId="57" state="hidden" r:id="rId41"/>
+    <sheet name="78" sheetId="53" state="hidden" r:id="rId42"/>
+    <sheet name="79" sheetId="55" state="hidden" r:id="rId43"/>
+    <sheet name="80" sheetId="58" state="hidden" r:id="rId44"/>
+    <sheet name="81" sheetId="59" state="hidden" r:id="rId45"/>
+    <sheet name="82" sheetId="60" state="hidden" r:id="rId46"/>
+    <sheet name="83" sheetId="62" state="hidden" r:id="rId47"/>
+    <sheet name="84" sheetId="65" state="hidden" r:id="rId48"/>
+    <sheet name="85" sheetId="67" state="hidden" r:id="rId49"/>
+    <sheet name="86" sheetId="69" r:id="rId50"/>
+    <sheet name="88" sheetId="71" r:id="rId51"/>
+    <sheet name="89" sheetId="72" r:id="rId52"/>
+    <sheet name="90" sheetId="73" r:id="rId53"/>
+    <sheet name="91" sheetId="74" r:id="rId54"/>
+    <sheet name="92" sheetId="75" r:id="rId55"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="38">'Aula 7'!$A$1:$I$25</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -74,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="434">
   <si>
     <t>Lista de Compras</t>
   </si>
@@ -1289,27 +1296,6 @@
     <t xml:space="preserve"> - Formatação Condicional</t>
   </si>
   <si>
-    <t>Relembrar tabela Dinamica</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -  Mostar Proprieda</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Nbão pode ter campos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Nostrar detalhes no numero</t>
-  </si>
-  <si>
-    <t>- Criar campo calculado</t>
-  </si>
-  <si>
-    <t>Demonstar CAMPO CALCULADo</t>
-  </si>
-  <si>
-    <t>Pedir para Calcular CAMPO CALCULADO</t>
-  </si>
-  <si>
     <t>Mostrar Conciliação</t>
   </si>
   <si>
@@ -1319,34 +1305,109 @@
     <t>Correção da Conciliação</t>
   </si>
   <si>
-    <t>Mostrar Grtafico Dinamico</t>
-  </si>
-  <si>
-    <t>Pedir Grafico Dinamicco</t>
-  </si>
-  <si>
     <t>Mostrar Conexão De dados Dinamica</t>
   </si>
   <si>
     <t>Pedir Demonstração simnples de conexão</t>
   </si>
   <si>
-    <t>Exercicios de DAshBoard1</t>
-  </si>
-  <si>
-    <t>Exercicios DashBoard2</t>
-  </si>
-  <si>
-    <t>Imposrtação Dinamica de Arquivo Externo</t>
-  </si>
-  <si>
-    <t>Exercicios Oiportação Externa</t>
-  </si>
-  <si>
-    <t>Mostrar Importação</t>
-  </si>
-  <si>
-    <t>Mostrar Impressão</t>
+    <t>rever tabela dinamica</t>
+  </si>
+  <si>
+    <t>Intervalo nomeado</t>
+  </si>
+  <si>
+    <t>Grafico dinamico</t>
+  </si>
+  <si>
+    <t>conectar tabelas dinamicas</t>
+  </si>
+  <si>
+    <t>Substituir dados extrerno p/ tabela dinamica</t>
+  </si>
+  <si>
+    <t>Dash Board</t>
+  </si>
+  <si>
+    <t>fazerem Dinamica: SOMA, Contagem e %Coluna</t>
+  </si>
+  <si>
+    <t>Mostrar Dinamica Arquivo Externo acima de 1 Milhão</t>
+  </si>
+  <si>
+    <t>Relembrar tabela Dinamica e intervalo nomeado</t>
+  </si>
+  <si>
+    <t>Pedir para Calcular CAMPO CALCULADO = Margem, Margem %</t>
+  </si>
+  <si>
+    <t>pedir Criar Campo calculado</t>
+  </si>
+  <si>
+    <t>Pedir Criar Dinamica direta do TXT e Substituir anomes / Criar Campo calculado e Linha calculada</t>
+  </si>
+  <si>
+    <t>Demonstraçaõ grafico Dinamico</t>
+  </si>
+  <si>
+    <t>Exercicio grafico Dinamico c/Conexão de dados</t>
+  </si>
+  <si>
+    <t>Enxcerramento.</t>
+  </si>
+  <si>
+    <t>Trabalhar em dashBoard Impressão</t>
+  </si>
+  <si>
+    <t>1 -  Relembrar PROCV (0 e 1),  DEPOIS o SE, DEPOIS TABELA DINAMICA</t>
+  </si>
+  <si>
+    <t>2 - CONVERTER EM TABELA</t>
+  </si>
+  <si>
+    <t>3 - ADICIONAR DEZEMBRO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mostrar Agrupamentos por DATA e EVOLUCAO.</t>
+  </si>
+  <si>
+    <t>NÃO MOSTRAR CAMPOS CALCULADOS</t>
+  </si>
+  <si>
+    <t>Demonstar CAMPO CALCULADo Venda - Imposto</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -  Mostrar DUPLO CLIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Pedir para Eles Resumo por Vendedor,  - Evolulção POR VENDEDOR e CALSSIFICAÇÂO</t>
+  </si>
+  <si>
+    <t>Arquivo VENDAS E MARGEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Demandar o Calculo usando PROCV, Fazer tabela Dinamica.</t>
+  </si>
+  <si>
+    <t>- EXPLICAR COMO ELE AGRUPA E DEPOIS CALCULA: USAR COMO EXEMPLO O %IMPOSTO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - PEDIR PARA CALCULAREM A MARGEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - PEDIR PARA CALCULAREM %MARGEM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - EXPLICAR CAMPO CALCULADO: usar como Exemplo a Receita LIQUIDA (Vendas - Imposto).</t>
+  </si>
+  <si>
+    <t>Arquivo VENDAS WEB x TOTVS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Pedirem para Fazer os calculos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Mostrar COMO usar dinamica para fazer conciliação.</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1458,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1470,6 +1531,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1483,7 +1550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1519,6 +1586,7 @@
     <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6506,21 +6574,24 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I48"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="80.28515625" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" style="15" customWidth="1"/>
     <col min="7" max="7" width="50.85546875" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2" s="15" t="s">
         <v>112</v>
       </c>
@@ -6528,7 +6599,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
@@ -6544,11 +6615,8 @@
       <c r="E3" t="s">
         <v>107</v>
       </c>
-      <c r="H3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>6.9444444444444753E-3</v>
       </c>
@@ -6568,11 +6636,8 @@
       <c r="F4" s="15">
         <v>75</v>
       </c>
-      <c r="I4">
-        <v>6.9444444444444198E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -6581,96 +6646,84 @@
         <v>0.3611111111111111</v>
       </c>
       <c r="C5" s="12">
-        <v>0.375</v>
+        <v>0.38194444444444442</v>
       </c>
       <c r="D5" s="12">
         <f t="shared" ref="D5:D19" si="1">C5-B5</f>
-        <v>1.3888888888888895E-2</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>409</v>
       </c>
       <c r="F5" s="15">
         <v>76</v>
       </c>
-      <c r="I5">
-        <v>6.9444444444444753E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>1.3888888888888951E-2</v>
       </c>
       <c r="B6" s="12">
         <f t="shared" si="0"/>
-        <v>0.375</v>
+        <v>0.38194444444444442</v>
       </c>
       <c r="C6" s="12">
-        <v>0.38541666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" si="1"/>
-        <v>1.0416666666666685E-2</v>
+        <v>1.3888888888888895E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="F6" s="15">
         <v>77</v>
       </c>
-      <c r="I6">
-        <v>2.0833333333333315E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="12">
         <f t="shared" si="0"/>
-        <v>0.38541666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C7" s="12">
-        <v>0.40277777777777773</v>
+        <v>0.40625</v>
       </c>
       <c r="D7" s="12">
         <f t="shared" si="1"/>
-        <v>1.7361111111111049E-2</v>
+        <v>1.0416666666666685E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="F7" s="15">
         <v>77</v>
       </c>
-      <c r="I7">
-        <v>6.9444444444444198E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B8" s="12">
         <f t="shared" si="0"/>
-        <v>0.40277777777777773</v>
+        <v>0.40625</v>
       </c>
       <c r="C8" s="12">
         <v>0.41666666666666669</v>
       </c>
       <c r="D8" s="12">
         <f t="shared" si="1"/>
-        <v>1.3888888888888951E-2</v>
+        <v>1.0416666666666685E-2</v>
       </c>
       <c r="E8" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="F8" s="15">
         <v>78</v>
       </c>
-      <c r="I8">
-        <v>2.083333333333337E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>6.9444444444444198E-3</v>
       </c>
@@ -6678,98 +6731,84 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="C9" s="12">
-        <v>0.4513888888888889</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="D9" s="12">
         <f t="shared" si="1"/>
-        <v>3.472222222222221E-2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>404</v>
-      </c>
+        <v>1.3888888888888895E-2</v>
+      </c>
+      <c r="E9" s="14"/>
       <c r="F9" s="15">
         <v>79</v>
       </c>
-      <c r="I9">
-        <v>6.9444444444444198E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B10" s="12">
         <f t="shared" si="0"/>
-        <v>0.4513888888888889</v>
+        <v>0.43055555555555558</v>
       </c>
       <c r="C10" s="12">
-        <v>0.45833333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="D10" s="12">
         <f>C10-B10</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="F10" s="15">
         <v>79</v>
       </c>
-      <c r="I10">
-        <v>2.0833333333333315E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B11" s="12">
         <f t="shared" si="0"/>
-        <v>0.45833333333333331</v>
+        <v>0.44444444444444442</v>
       </c>
       <c r="C11" s="12">
-        <v>0.46875</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="D11" s="12">
         <f t="shared" si="1"/>
-        <v>1.0416666666666685E-2</v>
+        <v>2.7777777777777846E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="F11" s="15">
         <v>79</v>
       </c>
-      <c r="I11">
-        <v>6.9444444444444753E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B12" s="12">
         <f t="shared" si="0"/>
-        <v>0.46875</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="C12" s="12">
         <v>0.48958333333333331</v>
       </c>
       <c r="D12" s="12">
         <f>C12-B12</f>
-        <v>2.0833333333333315E-2</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="E12" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="F12" s="15">
         <v>79</v>
       </c>
-      <c r="I12">
-        <v>0.13194444444444448</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>1.388888888888884E-2</v>
       </c>
@@ -6778,70 +6817,61 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="C13" s="12">
-        <v>0.54166666666666663</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="D13" s="12">
         <f t="shared" si="1"/>
-        <v>5.2083333333333315E-2</v>
+        <v>3.4722222222222654E-3</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>411</v>
       </c>
       <c r="F13" s="15">
         <v>81</v>
       </c>
-      <c r="I13">
-        <v>2.0833333333333259E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>1.3888888888888895E-2</v>
       </c>
       <c r="B14" s="12">
         <f t="shared" si="0"/>
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="C14" s="12">
         <v>0.54166666666666663</v>
-      </c>
-      <c r="C14" s="12">
-        <v>0.55208333333333337</v>
       </c>
       <c r="D14" s="12">
         <f t="shared" si="1"/>
-        <v>1.0416666666666741E-2</v>
+        <v>4.8611111111111049E-2</v>
       </c>
       <c r="E14" t="s">
-        <v>408</v>
-      </c>
-      <c r="I14">
-        <v>1.3888888888888951E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>6.9444444444444198E-3</v>
       </c>
       <c r="B15" s="12">
         <f t="shared" si="0"/>
-        <v>0.55208333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="C15" s="12">
         <v>0.5625</v>
       </c>
       <c r="D15" s="12">
         <f t="shared" si="1"/>
-        <v>1.041666666666663E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F15" s="15">
         <v>82</v>
       </c>
-      <c r="I15">
-        <v>2.083333333333337E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>1.0416666666666685E-2</v>
       </c>
@@ -6850,86 +6880,77 @@
         <v>0.5625</v>
       </c>
       <c r="C16" s="12">
-        <v>0.60416666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D16" s="12">
         <f t="shared" si="1"/>
-        <v>4.166666666666663E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="E16" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="F16" s="15">
         <v>82</v>
       </c>
-      <c r="I16">
-        <v>1.388888888888884E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>6.9444444444444753E-3</v>
       </c>
       <c r="B17" s="12">
         <f t="shared" si="0"/>
-        <v>0.60416666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C17" s="12">
-        <v>0.625</v>
+        <v>0.59722222222222221</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" si="1"/>
-        <v>2.083333333333337E-2</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
       <c r="F17" s="15">
         <v>83</v>
       </c>
-      <c r="I17">
-        <v>1.388888888888884E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B18" s="12">
         <f t="shared" si="0"/>
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C18" s="12">
         <v>0.625</v>
-      </c>
-      <c r="C18" s="12">
-        <v>0.63888888888888895</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="1"/>
-        <v>1.3888888888888951E-2</v>
+        <v>2.777777777777779E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="F18" s="15">
         <v>84</v>
       </c>
-      <c r="I18">
-        <v>2.083333333333337E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B19" s="12">
         <f t="shared" si="0"/>
+        <v>0.625</v>
+      </c>
+      <c r="C19" s="12">
         <v>0.63888888888888895</v>
-      </c>
-      <c r="C19" s="12">
-        <v>0.65972222222222221</v>
       </c>
       <c r="D19" s="12">
         <f t="shared" si="1"/>
-        <v>2.0833333333333259E-2</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="E19" t="s">
         <v>413</v>
@@ -6937,58 +6958,52 @@
       <c r="F19" s="15">
         <v>84</v>
       </c>
-      <c r="I19">
-        <v>1.388888888888884E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B20" s="12">
         <f>C19</f>
-        <v>0.65972222222222221</v>
+        <v>0.63888888888888895</v>
       </c>
       <c r="C20" s="12">
-        <v>0.66666666666666663</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="D20" s="12">
         <f>C20-B20</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.388888888888884E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>122</v>
+        <v>414</v>
       </c>
       <c r="F20" s="15">
         <v>84</v>
       </c>
-      <c r="I20">
-        <v>-2.083333333333337E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>2.4305555555555525E-2</v>
       </c>
       <c r="B21" s="12">
         <f>C20</f>
-        <v>0.66666666666666663</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="C21" s="12">
         <v>0.69444444444444453</v>
       </c>
       <c r="D21" s="12">
         <f>C21-B21</f>
-        <v>2.7777777777777901E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="E21" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="F21" s="15">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>2.4305555555555525E-2</v>
       </c>
@@ -7010,188 +7025,176 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-    </row>
-    <row r="32" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F31"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12" t="s">
-        <v>360</v>
-      </c>
-      <c r="E34" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="29" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="29" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="29" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="F37"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="29" t="s">
-        <v>336</v>
-      </c>
-      <c r="F38" s="15" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E39" s="29" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F38"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F39"/>
+      <c r="G39"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="F41" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+      <c r="F42" s="15">
+        <f>2*30</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>392</v>
+      </c>
+      <c r="F43" s="15">
+        <f>2*30</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>405</v>
+      </c>
+      <c r="F44" s="15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>404</v>
+      </c>
+      <c r="F45" s="15">
+        <f>3*30</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E46" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F46" s="15">
+        <f>3*30</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
-        <v>395</v>
+        <v>406</v>
+      </c>
+      <c r="F47" s="15">
+        <f>2*60</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="15">
+        <f>8*60</f>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="66" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7298,18 +7301,6 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
@@ -7351,7 +7342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7376,7 +7367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7409,7 +7400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7450,7 +7441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7482,7 +7473,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7532,7 +7523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7559,7 +7550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7677,12 +7668,60 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7790,7 +7829,21 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E15"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -7808,62 +7861,185 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>386</v>
       </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B6"/>
+  <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
-        <v>400</v>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>425</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>

</xml_diff>